<commit_message>
adding "Nobody IN" as reason for not interviewing
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/visit_registration.xlsx
+++ b/xforms/xlsforms/visit_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-195" windowWidth="15600" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-195" windowWidth="15600" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t>type</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>concat(${locationId},'_VISIT_',${visitId},'_',${fieldWorkerId})</t>
+  </si>
+  <si>
+    <t>Nobody IN</t>
   </si>
 </sst>
 </file>
@@ -1510,10 +1513,10 @@
   <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2209,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2367,20 +2370,28 @@
         <v>87</v>
       </c>
       <c r="B11" s="13">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="13">
         <v>99</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D12" s="14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
@@ -2727,7 +2738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added parameter autocalculated real visit (if the people are in house and "visited" gets value 0, otherwise 1)
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/visit_registration.xlsx
+++ b/xforms/xlsforms/visit_registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-195" windowWidth="15600" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-195" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
   <si>
     <t>type</t>
   </si>
@@ -339,7 +339,16 @@
     <t>concat(${locationId},'_VISIT_',${visitId},'_',${fieldWorkerId})</t>
   </si>
   <si>
-    <t>Nobody IN</t>
+    <t xml:space="preserve">Nobody to interview </t>
+  </si>
+  <si>
+    <t>realVisit</t>
+  </si>
+  <si>
+    <t>Real Visit</t>
+  </si>
+  <si>
+    <t>if(../correctInterviewee='1',0,if(../reason='88',1,0)))</t>
   </si>
 </sst>
 </file>
@@ -1510,13 +1519,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q90"/>
+  <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1936,38 +1945,41 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="M20" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1975,50 +1987,61 @@
       <c r="I21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L21" s="5" t="s">
+    </row>
+    <row r="22" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="I22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="M22" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="M23" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2040,16 +2063,16 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -2064,7 +2087,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2104,7 +2127,6 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
@@ -2134,6 +2156,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
@@ -2143,19 +2166,25 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I42" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I43" s="3"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I51" s="3"/>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I59" s="3"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="3"/>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I60" s="3"/>
@@ -2169,8 +2198,8 @@
     <row r="63" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I63" s="3"/>
     </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I80" s="3"/>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I64" s="3"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I81" s="3"/>
@@ -2185,7 +2214,6 @@
       <c r="I84" s="3"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
       <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -2197,10 +2225,14 @@
       <c r="I87" s="3"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="3"/>
       <c r="I88" s="3"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I90" s="3"/>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I89" s="3"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I91" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2212,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Slightly modified visit registration form to display input name of interviewee only if reason for interview is not 'nobody there to interview'
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/visit_registration.xlsx
+++ b/xforms/xlsforms/visit_registration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t>type</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>if(../correctInterviewee='1',0,if(../reason='88',1,0))</t>
+  </si>
+  <si>
+    <t>../correctInterviewee = '0' and not(selected(${reason}, '88'))</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +1528,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1906,17 +1909,17 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
+      <c r="A18" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I18" s="4" t="b">
         <v>1</v>
@@ -1925,24 +1928,24 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>90</v>
+    <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" s="4" t="b">
         <v>1</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
@@ -2245,7 +2248,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>